<commit_message>
Added Error Comments in RowMode
</commit_message>
<xml_diff>
--- a/toolkit.excel.test/TestWorkbooks/TestWB.xlsx
+++ b/toolkit.excel.test/TestWorkbooks/TestWB.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="138">
   <si>
     <t>name</t>
   </si>
@@ -421,6 +422,18 @@
   </si>
   <si>
     <t>filetable_updates_2105058535</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
   </si>
 </sst>
 </file>
@@ -744,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L108"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4857,4 +4870,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>